<commit_message>
cleaned notebook, ran kaggle bm and with my dataset
</commit_message>
<xml_diff>
--- a/capstone_project/sim_log.xlsx
+++ b/capstone_project/sim_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>simname</t>
   </si>
@@ -22,30 +22,23 @@
     <t>sim_desc</t>
   </si>
   <si>
-    <t>mine_initial</t>
-  </si>
-  <si>
-    <t>500_epochs</t>
-  </si>
-  <si>
-    <t>500_epoch_lookback_40</t>
-  </si>
-  <si>
-    <t>linear regression</t>
-  </si>
-  <si>
-    <t>kaggle params</t>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>kaggle_bm</t>
+  </si>
+  <si>
+    <t>kaggle param my dataset</t>
   </si>
   <si>
     <t xml:space="preserve">
-kaggle params but with 500 epochs to account for more features
-</t>
-  </si>
-  <si>
-    <t>500 iterations, lookback 40</t>
-  </si>
-  <si>
-    <t>1 row lookback</t>
+    kaggle params
+    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+    kaggle params with my dataset
+    </t>
   </si>
 </sst>
 </file>
@@ -403,7 +396,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -425,7 +418,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -436,7 +429,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -447,18 +440,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>